<commit_message>
Ultimas actuañizaciones del día de hoy
</commit_message>
<xml_diff>
--- a/Entenimiento_de_Datos/Diccionario.Bergamo.xlsx
+++ b/Entenimiento_de_Datos/Diccionario.Bergamo.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6466430e62763b8f/Desktop/Clonacion/Analitica_Datos/Analitica_Datos/Entenimiento_de_Datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{9E250304-FC16-4732-A188-D435D5897739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5AC4218-20C3-4B67-A8B7-5AA94A70D1DB}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="8_{9E250304-FC16-4732-A188-D435D5897739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB4F87B7-A1E1-4386-896D-EFD28BCC0383}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F6C894B3-B1CE-453B-A1A4-E4C084046781}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F6C894B3-B1CE-453B-A1A4-E4C084046781}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$13:$E$88</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="226">
   <si>
     <t>id</t>
   </si>
@@ -721,6 +724,12 @@
   </si>
   <si>
     <t>Asimismo, se incorporaron variables relacionadas con el desempeño y la profesionalización de los anfitriones, como antigüedad en la plataforma, nivel de verificación, estatus de superhost y cantidad de anuncios gestionados, lo que permite analizar su confiabilidad y estrategias de gestión. También se consideran indicadores de satisfacción de los huéspedes, como el número y frecuencia de reseñas y las calificaciones en limpieza, ubicación, comunicación y relación calidad-precio. Las variables geoespaciales y de vecindario, incluyendo coordenadas y barrios geocodificados, facilitan estudios de proximidad, segmentación por zonas y evaluación del impacto de la ubicación sobre precios, ocupación y experiencia del huésped. En conjunto, estas 50 variables proporcionan una base sólida para realizar un análisis completo del ecosistema Airbnb en Bergamo, ofreciendo información clave para la toma de decisiones estratégicas en la gestión de propiedades, optimización de precios y desarrollo de negocios turísticos.</t>
+  </si>
+  <si>
+    <t>object</t>
+  </si>
+  <si>
+    <t>float</t>
   </si>
 </sst>
 </file>
@@ -1405,8 +1414,8 @@
   </sheetPr>
   <dimension ref="A1:E88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:E9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="81" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1755,7 +1764,9 @@
       <c r="A29" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B29" s="6"/>
+      <c r="B29" s="6" t="s">
+        <v>224</v>
+      </c>
       <c r="C29" s="5" t="s">
         <v>104</v>
       </c>
@@ -1770,7 +1781,9 @@
       <c r="A30" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B30" s="6"/>
+      <c r="B30" s="6" t="s">
+        <v>224</v>
+      </c>
       <c r="C30" s="5" t="s">
         <v>104</v>
       </c>
@@ -1785,7 +1798,9 @@
       <c r="A31" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B31" s="6"/>
+      <c r="B31" s="6" t="s">
+        <v>224</v>
+      </c>
       <c r="C31" s="5"/>
       <c r="D31" s="13" t="s">
         <v>112</v>
@@ -1878,7 +1893,9 @@
       <c r="A38" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B38" s="6"/>
+      <c r="B38" s="6" t="s">
+        <v>224</v>
+      </c>
       <c r="C38" s="5" t="s">
         <v>104</v>
       </c>
@@ -2469,7 +2486,9 @@
       <c r="A75" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B75" s="6"/>
+      <c r="B75" s="6" t="s">
+        <v>225</v>
+      </c>
       <c r="C75" s="5" t="s">
         <v>104</v>
       </c>
@@ -2484,7 +2503,9 @@
       <c r="A76" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B76" s="6"/>
+      <c r="B76" s="6" t="s">
+        <v>225</v>
+      </c>
       <c r="C76" s="5" t="s">
         <v>104</v>
       </c>
@@ -2499,7 +2520,9 @@
       <c r="A77" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B77" s="6"/>
+      <c r="B77" s="6" t="s">
+        <v>225</v>
+      </c>
       <c r="C77" s="5" t="s">
         <v>104</v>
       </c>
@@ -2514,7 +2537,9 @@
       <c r="A78" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B78" s="6"/>
+      <c r="B78" s="6" t="s">
+        <v>225</v>
+      </c>
       <c r="C78" s="5" t="s">
         <v>104</v>
       </c>
@@ -2529,7 +2554,9 @@
       <c r="A79" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B79" s="6"/>
+      <c r="B79" s="6" t="s">
+        <v>225</v>
+      </c>
       <c r="C79" s="5" t="s">
         <v>104</v>
       </c>
@@ -2544,7 +2571,9 @@
       <c r="A80" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B80" s="6"/>
+      <c r="B80" s="6" t="s">
+        <v>225</v>
+      </c>
       <c r="C80" s="5" t="s">
         <v>104</v>
       </c>
@@ -2559,7 +2588,9 @@
       <c r="A81" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B81" s="6"/>
+      <c r="B81" s="6" t="s">
+        <v>225</v>
+      </c>
       <c r="C81" s="5" t="s">
         <v>104</v>
       </c>
@@ -2690,6 +2721,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A13:E88" xr:uid="{C594C5F6-0BC3-4241-9932-C1EF930E5A44}"/>
   <mergeCells count="7">
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="A12:E12"/>

</xml_diff>